<commit_message>
Updated backtest Excel file for weather analysis
</commit_message>
<xml_diff>
--- a/cfb_weather_backtest.xlsx
+++ b/cfb_weather_backtest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mckin\Dropbox\MS Docs\Work\Sublime_Misc\football_weather_repo\football_weather\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BB5E902-1526-4322-80CD-7345A09F789A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A0FAF65-03E3-44A3-86F0-6D33687AC655}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33015" yWindow="4410" windowWidth="18945" windowHeight="15345" activeTab="1" xr2:uid="{219F7BC0-C6D1-4389-8714-548F944ECF42}"/>
+    <workbookView xWindow="38295" yWindow="0" windowWidth="38610" windowHeight="20985" activeTab="1" xr2:uid="{219F7BC0-C6D1-4389-8714-548F944ECF42}"/>
   </bookViews>
   <sheets>
     <sheet name="Backtesting" sheetId="1" r:id="rId1"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="745" uniqueCount="368">
   <si>
     <t>Sport</t>
   </si>
@@ -1141,6 +1141,36 @@
   </si>
   <si>
     <t>5-3-0</t>
+  </si>
+  <si>
+    <t>Appalachian State</t>
+  </si>
+  <si>
+    <t>Kidd Brewer Stadium</t>
+  </si>
+  <si>
+    <t>9-5-0</t>
+  </si>
+  <si>
+    <t>Kennesaw State</t>
+  </si>
+  <si>
+    <t>Fifth Third Stadium</t>
+  </si>
+  <si>
+    <t>0-0-0</t>
+  </si>
+  <si>
+    <t>Jacksonville State</t>
+  </si>
+  <si>
+    <t>AmFirst Stadium</t>
+  </si>
+  <si>
+    <t>Aloha Stadium</t>
+  </si>
+  <si>
+    <t>Hawaii</t>
   </si>
 </sst>
 </file>
@@ -7064,10 +7094,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25DDF12B-BF75-4B96-8514-449138EF37C1}">
-  <dimension ref="A1:D118"/>
+  <dimension ref="A1:D122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
-      <selection activeCell="D123" sqref="D123"/>
+    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
+      <selection activeCell="I125" sqref="I125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8730,8 +8760,64 @@
         <v>0.193</v>
       </c>
     </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>358</v>
+      </c>
+      <c r="B119" t="s">
+        <v>359</v>
+      </c>
+      <c r="C119" s="25" t="s">
+        <v>360</v>
+      </c>
+      <c r="D119" s="24">
+        <v>0.214</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>361</v>
+      </c>
+      <c r="B120" t="s">
+        <v>362</v>
+      </c>
+      <c r="C120" s="25" t="s">
+        <v>363</v>
+      </c>
+      <c r="D120" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>364</v>
+      </c>
+      <c r="B121" t="s">
+        <v>365</v>
+      </c>
+      <c r="C121" s="25" t="s">
+        <v>363</v>
+      </c>
+      <c r="D121" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>367</v>
+      </c>
+      <c r="B122" t="s">
+        <v>366</v>
+      </c>
+      <c r="C122" s="25" t="s">
+        <v>363</v>
+      </c>
+      <c r="D122" s="24">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D118">
+  <conditionalFormatting sqref="D2:D122">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>